<commit_message>
Remove outdated boxplot image and update hiking data files to the latest versions.
</commit_message>
<xml_diff>
--- a/hiking_data_v2_updated.xlsx
+++ b/hiking_data_v2_updated.xlsx
@@ -758,7 +758,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -1559,7 +1559,7 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>Camera,Phone,Text messaging</t>
+          <t>Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>Musics,AllTrails,Camera,Text messaging</t>
+          <t>Audio, Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Text messaging</t>
+          <t>Maps, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr"/>
@@ -2698,7 +2698,7 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr"/>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr"/>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA21" t="inlineStr"/>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Phone</t>
+          <t>Maps, Audio, Phone</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr">
@@ -4119,7 +4119,7 @@
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr">
@@ -4284,7 +4284,7 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>Musics,AllTrails</t>
+          <t>Audio, Maps</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr"/>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr">
@@ -5435,7 +5435,7 @@
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>Camera,Text messaging</t>
+          <t>Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr"/>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>Musics,Text messaging</t>
+          <t>Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA35" t="inlineStr">
@@ -6248,7 +6248,7 @@
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA36" t="inlineStr">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>AllTrails,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA37" t="inlineStr"/>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>Maps,Phone,Text messaging</t>
+          <t>Maps, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA38" t="inlineStr"/>
@@ -6719,7 +6719,7 @@
       </c>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA39" t="inlineStr">
@@ -6880,7 +6880,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA40" t="inlineStr">
@@ -7037,7 +7037,7 @@
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA41" t="inlineStr"/>
@@ -7198,7 +7198,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA42" t="inlineStr">
@@ -7371,7 +7371,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA43" t="inlineStr">
@@ -7540,7 +7540,7 @@
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA44" t="inlineStr"/>
@@ -7693,7 +7693,7 @@
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA45" t="inlineStr"/>
@@ -7858,7 +7858,7 @@
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA46" t="inlineStr"/>
@@ -8325,7 +8325,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
@@ -8482,7 +8482,7 @@
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA50" t="inlineStr"/>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr"/>
@@ -8788,7 +8788,7 @@
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
@@ -8949,7 +8949,7 @@
       </c>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Social Media,Text messaging</t>
+          <t>Audio, Social Media, Text messaging</t>
         </is>
       </c>
       <c r="AA53" t="inlineStr">
@@ -9114,7 +9114,7 @@
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>Camera,Phone</t>
+          <t>Camera, Phone</t>
         </is>
       </c>
       <c r="AA54" t="inlineStr"/>
@@ -9267,7 +9267,7 @@
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Social Media,Text messaging</t>
+          <t>Maps, Audio, Social Media, Text messaging</t>
         </is>
       </c>
       <c r="AA55" t="inlineStr">
@@ -9436,7 +9436,7 @@
       </c>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA56" t="inlineStr">
@@ -9597,7 +9597,7 @@
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA57" t="inlineStr">
@@ -9758,7 +9758,7 @@
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA58" t="inlineStr">
@@ -9923,7 +9923,7 @@
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA59" t="inlineStr"/>
@@ -10088,7 +10088,7 @@
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>Podcast</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA60" t="inlineStr"/>
@@ -10394,7 +10394,7 @@
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>Social Media,Camera,Phone,Text messaging</t>
+          <t>Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA62" t="inlineStr"/>
@@ -10543,7 +10543,7 @@
       </c>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA63" t="inlineStr">
@@ -10696,7 +10696,7 @@
       </c>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>Social Media,Camera,Phone,Text messaging</t>
+          <t>Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA64" t="inlineStr"/>
@@ -10861,7 +10861,7 @@
       </c>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA65" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr"/>
@@ -11183,7 +11183,7 @@
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">
@@ -11348,7 +11348,7 @@
       </c>
       <c r="Z68" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA68" t="inlineStr">
@@ -11513,7 +11513,7 @@
       </c>
       <c r="Z69" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Text messaging</t>
+          <t>Maps, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA69" t="inlineStr"/>
@@ -11666,7 +11666,7 @@
       </c>
       <c r="Z70" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone</t>
+          <t>Maps, Audio, Social Media, Camera, Phone</t>
         </is>
       </c>
       <c r="AA70" t="inlineStr">
@@ -11839,7 +11839,7 @@
       </c>
       <c r="Z71" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA71" t="inlineStr">
@@ -12004,7 +12004,7 @@
       </c>
       <c r="Z72" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA72" t="inlineStr"/>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="Z73" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA73" t="inlineStr"/>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="Z74" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA74" t="inlineStr"/>
@@ -12487,7 +12487,7 @@
       </c>
       <c r="Z75" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA75" t="inlineStr">
@@ -12660,7 +12660,7 @@
       </c>
       <c r="Z76" t="inlineStr">
         <is>
-          <t>Maps,Musics</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA76" t="inlineStr">
@@ -12817,7 +12817,7 @@
       </c>
       <c r="Z77" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA77" t="inlineStr">
@@ -12978,7 +12978,7 @@
       </c>
       <c r="Z78" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Phone</t>
+          <t>Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA78" t="inlineStr">
@@ -13143,7 +13143,7 @@
       </c>
       <c r="Z79" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA79" t="inlineStr">
@@ -13324,7 +13324,7 @@
       </c>
       <c r="Z80" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA80" t="inlineStr"/>
@@ -13481,7 +13481,7 @@
       </c>
       <c r="Z81" t="inlineStr">
         <is>
-          <t>Camera,Text messaging</t>
+          <t>Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA81" t="inlineStr"/>
@@ -13650,7 +13650,7 @@
       </c>
       <c r="Z82" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA82" t="inlineStr">
@@ -13815,7 +13815,7 @@
       </c>
       <c r="Z83" t="inlineStr">
         <is>
-          <t>Podcast,Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA83" t="inlineStr">
@@ -13976,7 +13976,7 @@
       </c>
       <c r="Z84" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA84" t="inlineStr"/>
@@ -14141,7 +14141,7 @@
       </c>
       <c r="Z85" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA85" t="inlineStr">
@@ -14302,7 +14302,7 @@
       </c>
       <c r="Z86" t="inlineStr">
         <is>
-          <t>Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA86" t="inlineStr">
@@ -14608,7 +14608,7 @@
       </c>
       <c r="Z88" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA88" t="inlineStr">
@@ -14769,7 +14769,7 @@
       </c>
       <c r="Z89" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA89" t="inlineStr"/>
@@ -14922,7 +14922,7 @@
       </c>
       <c r="Z90" t="inlineStr">
         <is>
-          <t>Musics,Camera,Phone,Text messaging</t>
+          <t>Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA90" t="inlineStr">
@@ -15087,7 +15087,7 @@
       </c>
       <c r="Z91" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA91" t="inlineStr">
@@ -15558,7 +15558,7 @@
       </c>
       <c r="Z94" t="inlineStr">
         <is>
-          <t>Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA94" t="inlineStr">
@@ -15719,7 +15719,7 @@
       </c>
       <c r="Z95" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA95" t="inlineStr">
@@ -15884,7 +15884,7 @@
       </c>
       <c r="Z96" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Social Media,Camera,Text messaging</t>
+          <t>Maps, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA96" t="inlineStr"/>
@@ -16045,7 +16045,7 @@
       </c>
       <c r="Z97" t="inlineStr">
         <is>
-          <t>Camera,Phone,Text messaging</t>
+          <t>Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA97" t="inlineStr"/>
@@ -16210,7 +16210,7 @@
       </c>
       <c r="Z98" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA98" t="inlineStr">
@@ -16367,7 +16367,7 @@
       </c>
       <c r="Z99" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA99" t="inlineStr">
@@ -16677,7 +16677,7 @@
       </c>
       <c r="Z101" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA101" t="inlineStr"/>
@@ -16834,7 +16834,7 @@
       </c>
       <c r="Z102" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA102" t="inlineStr">
@@ -17003,7 +17003,7 @@
       </c>
       <c r="Z103" t="inlineStr">
         <is>
-          <t>Maps,Phone,Text messaging</t>
+          <t>Maps, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA103" t="inlineStr"/>
@@ -17172,7 +17172,7 @@
       </c>
       <c r="Z104" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Phone</t>
+          <t>Audio, Phone</t>
         </is>
       </c>
       <c r="AA104" t="inlineStr">
@@ -17329,7 +17329,7 @@
       </c>
       <c r="Z105" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA105" t="inlineStr">
@@ -17490,7 +17490,7 @@
       </c>
       <c r="Z106" t="inlineStr">
         <is>
-          <t>Maps,Musics,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA106" t="inlineStr">
@@ -17655,7 +17655,7 @@
       </c>
       <c r="Z107" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA107" t="inlineStr"/>
@@ -17812,7 +17812,7 @@
       </c>
       <c r="Z108" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA108" t="inlineStr">
@@ -17977,7 +17977,7 @@
       </c>
       <c r="Z109" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA109" t="inlineStr">
@@ -18138,7 +18138,7 @@
       </c>
       <c r="Z110" t="inlineStr">
         <is>
-          <t>Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Audio, Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA110" t="inlineStr">
@@ -18303,7 +18303,7 @@
       </c>
       <c r="Z111" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA111" t="inlineStr">
@@ -18468,7 +18468,7 @@
       </c>
       <c r="Z112" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA112" t="inlineStr">
@@ -18633,7 +18633,7 @@
       </c>
       <c r="Z113" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA113" t="inlineStr">
@@ -18806,7 +18806,7 @@
       </c>
       <c r="Z114" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA114" t="inlineStr">
@@ -18967,7 +18967,7 @@
       </c>
       <c r="Z115" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA115" t="inlineStr"/>
@@ -19128,7 +19128,7 @@
       </c>
       <c r="Z116" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA116" t="inlineStr">
@@ -19309,7 +19309,7 @@
       </c>
       <c r="Z117" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA117" t="inlineStr">
@@ -19466,7 +19466,7 @@
       </c>
       <c r="Z118" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA118" t="inlineStr">
@@ -19635,7 +19635,7 @@
       </c>
       <c r="Z119" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA119" t="inlineStr"/>
@@ -19796,7 +19796,7 @@
       </c>
       <c r="Z120" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA120" t="inlineStr">
@@ -19965,7 +19965,7 @@
       </c>
       <c r="Z121" t="inlineStr">
         <is>
-          <t>Musics,Phone</t>
+          <t>Audio, Phone</t>
         </is>
       </c>
       <c r="AA121" t="inlineStr">
@@ -20126,7 +20126,7 @@
       </c>
       <c r="Z122" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA122" t="inlineStr">
@@ -20299,7 +20299,7 @@
       </c>
       <c r="Z123" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA123" t="inlineStr">
@@ -20460,7 +20460,7 @@
       </c>
       <c r="Z124" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA124" t="inlineStr"/>
@@ -20621,7 +20621,7 @@
       </c>
       <c r="Z125" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA125" t="inlineStr"/>
@@ -20778,7 +20778,7 @@
       </c>
       <c r="Z126" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA126" t="inlineStr">
@@ -20959,7 +20959,7 @@
       </c>
       <c r="Z127" t="inlineStr">
         <is>
-          <t>Maps,Musics,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA127" t="inlineStr">
@@ -21120,7 +21120,7 @@
       </c>
       <c r="Z128" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA128" t="inlineStr">
@@ -21293,7 +21293,7 @@
       </c>
       <c r="Z129" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA129" t="inlineStr"/>
@@ -21446,7 +21446,7 @@
       </c>
       <c r="Z130" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA130" t="inlineStr"/>
@@ -21615,7 +21615,7 @@
       </c>
       <c r="Z131" t="inlineStr">
         <is>
-          <t>Social Media,Camera,Phone,Text messaging</t>
+          <t>Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA131" t="inlineStr">
@@ -21772,7 +21772,7 @@
       </c>
       <c r="Z132" t="inlineStr">
         <is>
-          <t>Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA132" t="inlineStr">
@@ -21929,7 +21929,7 @@
       </c>
       <c r="Z133" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA133" t="inlineStr">
@@ -22090,7 +22090,7 @@
       </c>
       <c r="Z134" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA134" t="inlineStr">
@@ -22412,7 +22412,7 @@
       </c>
       <c r="Z136" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA136" t="inlineStr">
@@ -22577,7 +22577,7 @@
       </c>
       <c r="Z137" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA137" t="inlineStr">
@@ -22742,7 +22742,7 @@
       </c>
       <c r="Z138" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA138" t="inlineStr">
@@ -22911,7 +22911,7 @@
       </c>
       <c r="Z139" t="inlineStr">
         <is>
-          <t>Musics,Text messaging</t>
+          <t>Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA139" t="inlineStr"/>
@@ -23072,7 +23072,7 @@
       </c>
       <c r="Z140" t="inlineStr">
         <is>
-          <t>Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA140" t="inlineStr">
@@ -23237,7 +23237,7 @@
       </c>
       <c r="Z141" t="inlineStr">
         <is>
-          <t>Social Media,Camera,Phone,Text messaging</t>
+          <t>Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA141" t="inlineStr"/>
@@ -23390,7 +23390,7 @@
       </c>
       <c r="Z142" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA142" t="inlineStr">
@@ -23551,7 +23551,7 @@
       </c>
       <c r="Z143" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA143" t="inlineStr"/>
@@ -23708,7 +23708,7 @@
       </c>
       <c r="Z144" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA144" t="inlineStr"/>
@@ -23873,7 +23873,7 @@
       </c>
       <c r="Z145" t="inlineStr">
         <is>
-          <t>Phone,Text messaging</t>
+          <t>Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA145" t="inlineStr"/>
@@ -24199,7 +24199,7 @@
       </c>
       <c r="Z147" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA147" t="inlineStr">
@@ -24364,7 +24364,7 @@
       </c>
       <c r="Z148" t="inlineStr">
         <is>
-          <t>Musics,Phone</t>
+          <t>Audio, Phone</t>
         </is>
       </c>
       <c r="AA148" t="inlineStr">
@@ -24537,7 +24537,7 @@
       </c>
       <c r="Z149" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA149" t="inlineStr">
@@ -24702,7 +24702,7 @@
       </c>
       <c r="Z150" t="inlineStr">
         <is>
-          <t>Maps,Phone</t>
+          <t>Maps, Phone</t>
         </is>
       </c>
       <c r="AA150" t="inlineStr"/>
@@ -25016,7 +25016,7 @@
       </c>
       <c r="Z152" t="inlineStr">
         <is>
-          <t>AllTrails</t>
+          <t>Maps</t>
         </is>
       </c>
       <c r="AA152" t="inlineStr"/>
@@ -25169,7 +25169,7 @@
       </c>
       <c r="Z153" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA153" t="inlineStr">
@@ -25644,7 +25644,7 @@
       </c>
       <c r="Z156" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA156" t="inlineStr">
@@ -25829,7 +25829,7 @@
       </c>
       <c r="Z157" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA157" t="inlineStr"/>
@@ -25990,7 +25990,7 @@
       </c>
       <c r="Z158" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA158" t="inlineStr"/>
@@ -26159,7 +26159,7 @@
       </c>
       <c r="Z159" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA159" t="inlineStr"/>
@@ -26328,7 +26328,7 @@
       </c>
       <c r="Z160" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA160" t="inlineStr">
@@ -26493,7 +26493,7 @@
       </c>
       <c r="Z161" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA161" t="inlineStr"/>
@@ -26807,7 +26807,7 @@
       </c>
       <c r="Z163" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA163" t="inlineStr"/>
@@ -26976,7 +26976,7 @@
       </c>
       <c r="Z164" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA164" t="inlineStr"/>
@@ -27141,7 +27141,7 @@
       </c>
       <c r="Z165" t="inlineStr">
         <is>
-          <t>Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA165" t="inlineStr"/>
@@ -27298,7 +27298,7 @@
       </c>
       <c r="Z166" t="inlineStr">
         <is>
-          <t>Maps,Musics,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA166" t="inlineStr">
@@ -27451,7 +27451,7 @@
       </c>
       <c r="Z167" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA167" t="inlineStr"/>
@@ -27761,7 +27761,7 @@
       </c>
       <c r="Z169" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA169" t="inlineStr">
@@ -27942,7 +27942,7 @@
       </c>
       <c r="Z170" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA170" t="inlineStr">
@@ -28095,7 +28095,7 @@
       </c>
       <c r="Z171" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA171" t="inlineStr">
@@ -28409,7 +28409,7 @@
       </c>
       <c r="Z173" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA173" t="inlineStr">
@@ -28574,7 +28574,7 @@
       </c>
       <c r="Z174" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA174" t="inlineStr">
@@ -28727,7 +28727,7 @@
       </c>
       <c r="Z175" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA175" t="inlineStr">
@@ -28896,7 +28896,7 @@
       </c>
       <c r="Z176" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA176" t="inlineStr"/>
@@ -29061,7 +29061,7 @@
       </c>
       <c r="Z177" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Phone</t>
+          <t>Maps, Audio, Phone</t>
         </is>
       </c>
       <c r="AA177" t="inlineStr">
@@ -29226,7 +29226,7 @@
       </c>
       <c r="Z178" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA178" t="inlineStr">
@@ -29391,7 +29391,7 @@
       </c>
       <c r="Z179" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA179" t="inlineStr">
@@ -29556,7 +29556,7 @@
       </c>
       <c r="Z180" t="inlineStr">
         <is>
-          <t>AllTrails,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA180" t="inlineStr"/>
@@ -29717,7 +29717,7 @@
       </c>
       <c r="Z181" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA181" t="inlineStr"/>
@@ -29870,7 +29870,7 @@
       </c>
       <c r="Z182" t="inlineStr">
         <is>
-          <t>Musics,AllTrails,Camera,Text messaging</t>
+          <t>Audio, Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA182" t="inlineStr">
@@ -30027,7 +30027,7 @@
       </c>
       <c r="Z183" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA183" t="inlineStr">
@@ -30196,7 +30196,7 @@
       </c>
       <c r="Z184" t="inlineStr">
         <is>
-          <t>Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA184" t="inlineStr">
@@ -30349,7 +30349,7 @@
       </c>
       <c r="Z185" t="inlineStr">
         <is>
-          <t>Phone,Text messaging</t>
+          <t>Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA185" t="inlineStr"/>
@@ -30502,7 +30502,7 @@
       </c>
       <c r="Z186" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA186" t="inlineStr"/>
@@ -30651,7 +30651,7 @@
       </c>
       <c r="Z187" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA187" t="inlineStr"/>
@@ -30800,7 +30800,7 @@
       </c>
       <c r="Z188" t="inlineStr">
         <is>
-          <t>Musics,Camera,Phone,Text messaging</t>
+          <t>Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA188" t="inlineStr">
@@ -30981,7 +30981,7 @@
       </c>
       <c r="Z189" t="inlineStr">
         <is>
-          <t>Maps,AllTrails</t>
+          <t>Maps</t>
         </is>
       </c>
       <c r="AA189" t="inlineStr"/>
@@ -31138,7 +31138,7 @@
       </c>
       <c r="Z190" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA190" t="inlineStr">
@@ -31299,7 +31299,7 @@
       </c>
       <c r="Z191" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA191" t="inlineStr">
@@ -31464,7 +31464,7 @@
       </c>
       <c r="Z192" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA192" t="inlineStr">
@@ -31621,7 +31621,7 @@
       </c>
       <c r="Z193" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA193" t="inlineStr"/>
@@ -31786,7 +31786,7 @@
       </c>
       <c r="Z194" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA194" t="inlineStr"/>
@@ -31947,7 +31947,7 @@
       </c>
       <c r="Z195" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA195" t="inlineStr"/>
@@ -32096,7 +32096,7 @@
       </c>
       <c r="Z196" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA196" t="inlineStr"/>
@@ -32241,7 +32241,7 @@
       </c>
       <c r="Z197" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA197" t="inlineStr"/>
@@ -32390,7 +32390,7 @@
       </c>
       <c r="Z198" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA198" t="inlineStr">
@@ -32555,7 +32555,7 @@
       </c>
       <c r="Z199" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA199" t="inlineStr">
@@ -32712,7 +32712,7 @@
       </c>
       <c r="Z200" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Social Media,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA200" t="inlineStr">
@@ -32869,7 +32869,7 @@
       </c>
       <c r="Z201" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA201" t="inlineStr"/>
@@ -33022,7 +33022,7 @@
       </c>
       <c r="Z202" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA202" t="inlineStr">
@@ -33183,7 +33183,7 @@
       </c>
       <c r="Z203" t="inlineStr">
         <is>
-          <t>Musics,Phone,Text messaging</t>
+          <t>Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA203" t="inlineStr">
@@ -33340,7 +33340,7 @@
       </c>
       <c r="Z204" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA204" t="inlineStr">
@@ -33497,7 +33497,7 @@
       </c>
       <c r="Z205" t="inlineStr">
         <is>
-          <t>Maps,Podcast</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA205" t="inlineStr">
@@ -33654,7 +33654,7 @@
       </c>
       <c r="Z206" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA206" t="inlineStr">
@@ -33827,7 +33827,7 @@
       </c>
       <c r="Z207" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA207" t="inlineStr">
@@ -34133,7 +34133,7 @@
       </c>
       <c r="Z209" t="inlineStr">
         <is>
-          <t>Camera,Text messaging</t>
+          <t>Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA209" t="inlineStr"/>
@@ -34290,7 +34290,7 @@
       </c>
       <c r="Z210" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA210" t="inlineStr"/>
@@ -34447,7 +34447,7 @@
       </c>
       <c r="Z211" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA211" t="inlineStr">
@@ -34785,7 +34785,7 @@
       </c>
       <c r="Z213" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA213" t="inlineStr">
@@ -34942,7 +34942,7 @@
       </c>
       <c r="Z214" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA214" t="inlineStr"/>
@@ -35107,7 +35107,7 @@
       </c>
       <c r="Z215" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA215" t="inlineStr"/>
@@ -35264,7 +35264,7 @@
       </c>
       <c r="Z216" t="inlineStr">
         <is>
-          <t>Podcast,Musics,AllTrails,Camera</t>
+          <t>Audio, Maps, Camera</t>
         </is>
       </c>
       <c r="AA216" t="inlineStr">
@@ -35425,7 +35425,7 @@
       </c>
       <c r="Z217" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA217" t="inlineStr">
@@ -35586,7 +35586,7 @@
       </c>
       <c r="Z218" t="inlineStr">
         <is>
-          <t>AllTrails,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA218" t="inlineStr"/>
@@ -35739,7 +35739,7 @@
       </c>
       <c r="Z219" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA219" t="inlineStr">
@@ -35912,7 +35912,7 @@
       </c>
       <c r="Z220" t="inlineStr">
         <is>
-          <t>Maps,AllTrails</t>
+          <t>Maps</t>
         </is>
       </c>
       <c r="AA220" t="inlineStr">
@@ -36073,7 +36073,7 @@
       </c>
       <c r="Z221" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA221" t="inlineStr">
@@ -36383,7 +36383,7 @@
       </c>
       <c r="Z223" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA223" t="inlineStr">
@@ -36548,7 +36548,7 @@
       </c>
       <c r="Z224" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA224" t="inlineStr">
@@ -36705,7 +36705,7 @@
       </c>
       <c r="Z225" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA225" t="inlineStr"/>
@@ -36858,7 +36858,7 @@
       </c>
       <c r="Z226" t="inlineStr">
         <is>
-          <t>Camera,Text messaging</t>
+          <t>Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA226" t="inlineStr">
@@ -37015,7 +37015,7 @@
       </c>
       <c r="Z227" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA227" t="inlineStr"/>
@@ -37168,7 +37168,7 @@
       </c>
       <c r="Z228" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA228" t="inlineStr">
@@ -37325,7 +37325,7 @@
       </c>
       <c r="Z229" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA229" t="inlineStr"/>
@@ -37478,7 +37478,7 @@
       </c>
       <c r="Z230" t="inlineStr">
         <is>
-          <t>Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA230" t="inlineStr">
@@ -37639,7 +37639,7 @@
       </c>
       <c r="Z231" t="inlineStr">
         <is>
-          <t>Musics,Phone,Text messaging</t>
+          <t>Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA231" t="inlineStr">
@@ -37796,7 +37796,7 @@
       </c>
       <c r="Z232" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA232" t="inlineStr"/>
@@ -37949,7 +37949,7 @@
       </c>
       <c r="Z233" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA233" t="inlineStr"/>
@@ -38102,7 +38102,7 @@
       </c>
       <c r="Z234" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA234" t="inlineStr">
@@ -38424,7 +38424,7 @@
       </c>
       <c r="Z236" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA236" t="inlineStr">
@@ -38577,7 +38577,7 @@
       </c>
       <c r="Z237" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Text messaging</t>
+          <t>Maps, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA237" t="inlineStr"/>
@@ -38726,7 +38726,7 @@
       </c>
       <c r="Z238" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA238" t="inlineStr"/>
@@ -38887,7 +38887,7 @@
       </c>
       <c r="Z239" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA239" t="inlineStr">
@@ -39052,7 +39052,7 @@
       </c>
       <c r="Z240" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA240" t="inlineStr"/>
@@ -39201,7 +39201,7 @@
       </c>
       <c r="Z241" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA241" t="inlineStr">
@@ -39358,7 +39358,7 @@
       </c>
       <c r="Z242" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA242" t="inlineStr"/>
@@ -39523,7 +39523,7 @@
       </c>
       <c r="Z243" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA243" t="inlineStr"/>
@@ -39684,7 +39684,7 @@
       </c>
       <c r="Z244" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA244" t="inlineStr">
@@ -39861,7 +39861,7 @@
       </c>
       <c r="Z245" t="inlineStr">
         <is>
-          <t>Phone,Text messaging</t>
+          <t>Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA245" t="inlineStr"/>
@@ -40018,7 +40018,7 @@
       </c>
       <c r="Z246" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA246" t="inlineStr">
@@ -40187,7 +40187,7 @@
       </c>
       <c r="Z247" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA247" t="inlineStr">
@@ -40352,7 +40352,7 @@
       </c>
       <c r="Z248" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA248" t="inlineStr">
@@ -40666,7 +40666,7 @@
       </c>
       <c r="Z250" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA250" t="inlineStr">
@@ -40827,7 +40827,7 @@
       </c>
       <c r="Z251" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA251" t="inlineStr">
@@ -40980,7 +40980,7 @@
       </c>
       <c r="Z252" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA252" t="inlineStr"/>
@@ -41133,7 +41133,7 @@
       </c>
       <c r="Z253" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA253" t="inlineStr">
@@ -41290,7 +41290,7 @@
       </c>
       <c r="Z254" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Text messaging</t>
+          <t>Maps, Audio, Social Media, Text messaging</t>
         </is>
       </c>
       <c r="AA254" t="inlineStr">
@@ -41471,7 +41471,7 @@
       </c>
       <c r="Z255" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA255" t="inlineStr">
@@ -41656,7 +41656,7 @@
       </c>
       <c r="Z256" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA256" t="inlineStr"/>
@@ -41809,7 +41809,7 @@
       </c>
       <c r="Z257" t="inlineStr">
         <is>
-          <t>Maps,Text messaging</t>
+          <t>Maps, Text messaging</t>
         </is>
       </c>
       <c r="AA257" t="inlineStr">
@@ -41970,7 +41970,7 @@
       </c>
       <c r="Z258" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA258" t="inlineStr">
@@ -42131,7 +42131,7 @@
       </c>
       <c r="Z259" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA259" t="inlineStr">
@@ -42300,7 +42300,7 @@
       </c>
       <c r="Z260" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA260" t="inlineStr"/>
@@ -42453,7 +42453,7 @@
       </c>
       <c r="Z261" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA261" t="inlineStr">
@@ -42630,7 +42630,7 @@
       </c>
       <c r="Z262" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA262" t="inlineStr">
@@ -42783,7 +42783,7 @@
       </c>
       <c r="Z263" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA263" t="inlineStr"/>
@@ -42936,7 +42936,7 @@
       </c>
       <c r="Z264" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA264" t="inlineStr">
@@ -43093,7 +43093,7 @@
       </c>
       <c r="Z265" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera</t>
+          <t>Maps, Social Media, Camera</t>
         </is>
       </c>
       <c r="AA265" t="inlineStr"/>
@@ -43266,7 +43266,7 @@
       </c>
       <c r="Z266" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA266" t="inlineStr">
@@ -43427,7 +43427,7 @@
       </c>
       <c r="Z267" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA267" t="inlineStr">
@@ -43612,7 +43612,7 @@
       </c>
       <c r="Z268" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA268" t="inlineStr">
@@ -43769,7 +43769,7 @@
       </c>
       <c r="Z269" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA269" t="inlineStr"/>
@@ -43926,7 +43926,7 @@
       </c>
       <c r="Z270" t="inlineStr">
         <is>
-          <t>AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA270" t="inlineStr"/>
@@ -44079,7 +44079,7 @@
       </c>
       <c r="Z271" t="inlineStr">
         <is>
-          <t>Maps,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA271" t="inlineStr"/>
@@ -44236,7 +44236,7 @@
       </c>
       <c r="Z272" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA272" t="inlineStr">
@@ -44393,7 +44393,7 @@
       </c>
       <c r="Z273" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA273" t="inlineStr">
@@ -44558,7 +44558,7 @@
       </c>
       <c r="Z274" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA274" t="inlineStr">
@@ -44719,7 +44719,7 @@
       </c>
       <c r="Z275" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA275" t="inlineStr">
@@ -44876,7 +44876,7 @@
       </c>
       <c r="Z276" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA276" t="inlineStr"/>
@@ -45045,7 +45045,7 @@
       </c>
       <c r="Z277" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA277" t="inlineStr">
@@ -45214,7 +45214,7 @@
       </c>
       <c r="Z278" t="inlineStr">
         <is>
-          <t>Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA278" t="inlineStr"/>
@@ -45524,7 +45524,7 @@
       </c>
       <c r="Z280" t="inlineStr">
         <is>
-          <t>Maps,Camera,Text messaging</t>
+          <t>Maps, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA280" t="inlineStr">
@@ -45681,7 +45681,7 @@
       </c>
       <c r="Z281" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA281" t="inlineStr"/>
@@ -45842,7 +45842,7 @@
       </c>
       <c r="Z282" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA282" t="inlineStr">
@@ -46149,7 +46149,7 @@
       </c>
       <c r="Z284" t="inlineStr">
         <is>
-          <t>Camera,Phone,Text messaging</t>
+          <t>Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA284" t="inlineStr">
@@ -46334,7 +46334,7 @@
       </c>
       <c r="Z285" t="inlineStr">
         <is>
-          <t>Camera,Phone,Text messaging</t>
+          <t>Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA285" t="inlineStr"/>
@@ -46499,7 +46499,7 @@
       </c>
       <c r="Z286" t="inlineStr">
         <is>
-          <t>Maps,Musics,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA286" t="inlineStr">
@@ -46660,7 +46660,7 @@
       </c>
       <c r="Z287" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA287" t="inlineStr"/>
@@ -46962,7 +46962,7 @@
       </c>
       <c r="Z289" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA289" t="inlineStr"/>
@@ -47115,7 +47115,7 @@
       </c>
       <c r="Z290" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA290" t="inlineStr">
@@ -47272,7 +47272,7 @@
       </c>
       <c r="Z291" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA291" t="inlineStr"/>
@@ -47429,7 +47429,7 @@
       </c>
       <c r="Z292" t="inlineStr">
         <is>
-          <t>Musics,Phone,Text messaging</t>
+          <t>Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA292" t="inlineStr">
@@ -47586,7 +47586,7 @@
       </c>
       <c r="Z293" t="inlineStr">
         <is>
-          <t>Musics,Phone,Text messaging</t>
+          <t>Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA293" t="inlineStr">
@@ -47763,7 +47763,7 @@
       </c>
       <c r="Z294" t="inlineStr">
         <is>
-          <t>Musics,Camera,Phone,Text messaging</t>
+          <t>Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA294" t="inlineStr">
@@ -47928,7 +47928,7 @@
       </c>
       <c r="Z295" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA295" t="inlineStr"/>
@@ -48097,7 +48097,7 @@
       </c>
       <c r="Z296" t="inlineStr">
         <is>
-          <t>Musics</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA296" t="inlineStr">
@@ -48258,7 +48258,7 @@
       </c>
       <c r="Z297" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA297" t="inlineStr">
@@ -48403,7 +48403,7 @@
       </c>
       <c r="Z298" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA298" t="inlineStr"/>
@@ -48556,7 +48556,7 @@
       </c>
       <c r="Z299" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA299" t="inlineStr">
@@ -48709,7 +48709,7 @@
       </c>
       <c r="Z300" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA300" t="inlineStr"/>
@@ -48862,7 +48862,7 @@
       </c>
       <c r="Z301" t="inlineStr">
         <is>
-          <t>Camera,Phone,None</t>
+          <t>Camera, Phone, None</t>
         </is>
       </c>
       <c r="AA301" t="inlineStr"/>
@@ -49015,7 +49015,7 @@
       </c>
       <c r="Z302" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA302" t="inlineStr">
@@ -49164,7 +49164,7 @@
       </c>
       <c r="Z303" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA303" t="inlineStr"/>
@@ -49313,7 +49313,7 @@
       </c>
       <c r="Z304" t="inlineStr">
         <is>
-          <t>Maps,AllTrails</t>
+          <t>Maps</t>
         </is>
       </c>
       <c r="AA304" t="inlineStr">
@@ -49490,7 +49490,7 @@
       </c>
       <c r="Z305" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera</t>
+          <t>Maps, Audio, Social Media, Camera</t>
         </is>
       </c>
       <c r="AA305" t="inlineStr">
@@ -49643,7 +49643,7 @@
       </c>
       <c r="Z306" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA306" t="inlineStr"/>
@@ -49800,7 +49800,7 @@
       </c>
       <c r="Z307" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA307" t="inlineStr">
@@ -49973,7 +49973,7 @@
       </c>
       <c r="Z308" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA308" t="inlineStr">
@@ -50283,7 +50283,7 @@
       </c>
       <c r="Z310" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA310" t="inlineStr">
@@ -50613,7 +50613,7 @@
       </c>
       <c r="Z312" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA312" t="inlineStr">
@@ -50770,7 +50770,7 @@
       </c>
       <c r="Z313" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Phone</t>
+          <t>Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA313" t="inlineStr">
@@ -50935,7 +50935,7 @@
       </c>
       <c r="Z314" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA314" t="inlineStr"/>
@@ -51229,7 +51229,7 @@
       </c>
       <c r="Z316" t="inlineStr">
         <is>
-          <t>Podcast,Phone</t>
+          <t>Audio, Phone</t>
         </is>
       </c>
       <c r="AA316" t="inlineStr"/>
@@ -51382,7 +51382,7 @@
       </c>
       <c r="Z317" t="inlineStr">
         <is>
-          <t>Maps,Musics,Phone</t>
+          <t>Maps, Audio, Phone</t>
         </is>
       </c>
       <c r="AA317" t="inlineStr"/>
@@ -51543,7 +51543,7 @@
       </c>
       <c r="Z318" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Phone,Text messaging</t>
+          <t>Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA318" t="inlineStr">
@@ -51704,7 +51704,7 @@
       </c>
       <c r="Z319" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA319" t="inlineStr">
@@ -51865,7 +51865,7 @@
       </c>
       <c r="Z320" t="inlineStr">
         <is>
-          <t>Maps,Musics,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA320" t="inlineStr">
@@ -52195,7 +52195,7 @@
       </c>
       <c r="Z322" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Text messaging</t>
+          <t>Maps, Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA322" t="inlineStr">
@@ -52348,7 +52348,7 @@
       </c>
       <c r="Z323" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA323" t="inlineStr">
@@ -52517,7 +52517,7 @@
       </c>
       <c r="Z324" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA324" t="inlineStr">
@@ -52682,7 +52682,7 @@
       </c>
       <c r="Z325" t="inlineStr">
         <is>
-          <t>Maps,AllTrails</t>
+          <t>Maps</t>
         </is>
       </c>
       <c r="AA325" t="inlineStr"/>
@@ -52835,7 +52835,7 @@
       </c>
       <c r="Z326" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Social Media,Camera,Text messaging</t>
+          <t>Maps, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA326" t="inlineStr"/>
@@ -52997,7 +52997,7 @@
       </c>
       <c r="Z327" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA327" t="inlineStr">
@@ -53162,7 +53162,7 @@
       </c>
       <c r="Z328" t="inlineStr">
         <is>
-          <t>Podcast,Phone</t>
+          <t>Audio, Phone</t>
         </is>
       </c>
       <c r="AA328" t="inlineStr">
@@ -53468,7 +53468,7 @@
       </c>
       <c r="Z330" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA330" t="inlineStr">
@@ -53633,7 +53633,7 @@
       </c>
       <c r="Z331" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA331" t="inlineStr">
@@ -53790,7 +53790,7 @@
       </c>
       <c r="Z332" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera</t>
+          <t>Maps, Audio, Social Media, Camera</t>
         </is>
       </c>
       <c r="AA332" t="inlineStr"/>
@@ -53951,7 +53951,7 @@
       </c>
       <c r="Z333" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA333" t="inlineStr"/>
@@ -54134,7 +54134,7 @@
       </c>
       <c r="Z334" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA334" t="inlineStr">
@@ -54291,7 +54291,7 @@
       </c>
       <c r="Z335" t="inlineStr">
         <is>
-          <t>AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA335" t="inlineStr"/>
@@ -54456,7 +54456,7 @@
       </c>
       <c r="Z336" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA336" t="inlineStr">
@@ -54625,7 +54625,7 @@
       </c>
       <c r="Z337" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA337" t="inlineStr">
@@ -54798,7 +54798,7 @@
       </c>
       <c r="Z338" t="inlineStr">
         <is>
-          <t>Maps,Musics</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA338" t="inlineStr">
@@ -54959,7 +54959,7 @@
       </c>
       <c r="Z339" t="inlineStr">
         <is>
-          <t>Podcast</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="AA339" t="inlineStr">
@@ -55126,7 +55126,7 @@
       </c>
       <c r="Z340" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA340" t="inlineStr">
@@ -55315,7 +55315,7 @@
       </c>
       <c r="Z341" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone,Text messaging</t>
+          <t>Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA341" t="inlineStr"/>
@@ -55468,7 +55468,7 @@
       </c>
       <c r="Z342" t="inlineStr">
         <is>
-          <t>Maps,Musics,Phone,Text messaging</t>
+          <t>Maps, Audio, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA342" t="inlineStr"/>
@@ -55621,7 +55621,7 @@
       </c>
       <c r="Z343" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA343" t="inlineStr">
@@ -55794,7 +55794,7 @@
       </c>
       <c r="Z344" t="inlineStr">
         <is>
-          <t>Camera,Text messaging</t>
+          <t>Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA344" t="inlineStr"/>
@@ -55943,7 +55943,7 @@
       </c>
       <c r="Z345" t="inlineStr">
         <is>
-          <t>Maps,Musics,AllTrails,Camera,Text messaging</t>
+          <t>Maps, Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA345" t="inlineStr">
@@ -56096,7 +56096,7 @@
       </c>
       <c r="Z346" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA346" t="inlineStr">
@@ -56253,7 +56253,7 @@
       </c>
       <c r="Z347" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA347" t="inlineStr">
@@ -56414,7 +56414,7 @@
       </c>
       <c r="Z348" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA348" t="inlineStr">
@@ -56708,7 +56708,7 @@
       </c>
       <c r="Z350" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA350" t="inlineStr">
@@ -56881,7 +56881,7 @@
       </c>
       <c r="Z351" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera</t>
+          <t>Maps, Audio, Camera</t>
         </is>
       </c>
       <c r="AA351" t="inlineStr">
@@ -57034,7 +57034,7 @@
       </c>
       <c r="Z352" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA352" t="inlineStr">
@@ -57191,7 +57191,7 @@
       </c>
       <c r="Z353" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA353" t="inlineStr">
@@ -57360,7 +57360,7 @@
       </c>
       <c r="Z354" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA354" t="inlineStr">
@@ -57547,7 +57547,7 @@
       </c>
       <c r="Z355" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA355" t="inlineStr">
@@ -57700,7 +57700,7 @@
       </c>
       <c r="Z356" t="inlineStr">
         <is>
-          <t>Musics,Social Media,Camera,Text messaging</t>
+          <t>Audio, Social Media, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA356" t="inlineStr"/>
@@ -58159,7 +58159,7 @@
       </c>
       <c r="Z359" t="inlineStr">
         <is>
-          <t>Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA359" t="inlineStr"/>
@@ -58312,7 +58312,7 @@
       </c>
       <c r="Z360" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA360" t="inlineStr">
@@ -58477,7 +58477,7 @@
       </c>
       <c r="Z361" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA361" t="inlineStr"/>
@@ -58646,7 +58646,7 @@
       </c>
       <c r="Z362" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails</t>
+          <t>Maps, Audio</t>
         </is>
       </c>
       <c r="AA362" t="inlineStr">
@@ -58807,7 +58807,7 @@
       </c>
       <c r="Z363" t="inlineStr">
         <is>
-          <t>Maps,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA363" t="inlineStr">
@@ -58976,7 +58976,7 @@
       </c>
       <c r="Z364" t="inlineStr">
         <is>
-          <t>Social Media,Camera,Phone,Text messaging</t>
+          <t>Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA364" t="inlineStr"/>
@@ -59137,7 +59137,7 @@
       </c>
       <c r="Z365" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA365" t="inlineStr"/>
@@ -59290,7 +59290,7 @@
       </c>
       <c r="Z366" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA366" t="inlineStr">
@@ -59443,7 +59443,7 @@
       </c>
       <c r="Z367" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,AllTrails,Social Media,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA367" t="inlineStr">
@@ -59769,7 +59769,7 @@
       </c>
       <c r="Z369" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Text messaging</t>
+          <t>Maps, Social Media, Text messaging</t>
         </is>
       </c>
       <c r="AA369" t="inlineStr"/>
@@ -59926,7 +59926,7 @@
       </c>
       <c r="Z370" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera,Text messaging</t>
+          <t>Audio, Camera, Text messaging</t>
         </is>
       </c>
       <c r="AA370" t="inlineStr">
@@ -60083,7 +60083,7 @@
       </c>
       <c r="Z371" t="inlineStr">
         <is>
-          <t>Maps,AllTrails,Camera</t>
+          <t>Maps, Camera</t>
         </is>
       </c>
       <c r="AA371" t="inlineStr"/>
@@ -60236,7 +60236,7 @@
       </c>
       <c r="Z372" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Text messaging</t>
+          <t>Audio, Text messaging</t>
         </is>
       </c>
       <c r="AA372" t="inlineStr">
@@ -60558,7 +60558,7 @@
       </c>
       <c r="Z374" t="inlineStr">
         <is>
-          <t>Podcast,Musics,Camera</t>
+          <t>Audio, Camera</t>
         </is>
       </c>
       <c r="AA374" t="inlineStr">
@@ -60856,7 +60856,7 @@
       </c>
       <c r="Z376" t="inlineStr">
         <is>
-          <t>Maps,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA376" t="inlineStr"/>
@@ -61013,7 +61013,7 @@
       </c>
       <c r="Z377" t="inlineStr">
         <is>
-          <t>AllTrails,Camera,Phone</t>
+          <t>Maps, Camera, Phone</t>
         </is>
       </c>
       <c r="AA377" t="inlineStr"/>
@@ -61166,7 +61166,7 @@
       </c>
       <c r="Z378" t="inlineStr">
         <is>
-          <t>Maps,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA378" t="inlineStr"/>
@@ -61335,7 +61335,7 @@
       </c>
       <c r="Z379" t="inlineStr">
         <is>
-          <t>Maps,Musics,Camera,Phone</t>
+          <t>Maps, Audio, Camera, Phone</t>
         </is>
       </c>
       <c r="AA379" t="inlineStr"/>
@@ -61508,7 +61508,7 @@
       </c>
       <c r="Z380" t="inlineStr">
         <is>
-          <t>Podcast,Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Audio, Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA380" t="inlineStr">
@@ -61814,7 +61814,7 @@
       </c>
       <c r="Z382" t="inlineStr">
         <is>
-          <t>Maps,Podcast,Musics,Social Media,Camera,Phone,Text messaging</t>
+          <t>Maps, Audio, Social Media, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA382" t="inlineStr">
@@ -61975,7 +61975,7 @@
       </c>
       <c r="Z383" t="inlineStr">
         <is>
-          <t>Musics,AllTrails,Camera,Phone,Text messaging</t>
+          <t>Audio, Maps, Camera, Phone, Text messaging</t>
         </is>
       </c>
       <c r="AA383" t="inlineStr">

</xml_diff>